<commit_message>
refactored and ran analysis on 3 pairs
</commit_message>
<xml_diff>
--- a/Data/Data admin.xlsx
+++ b/Data/Data admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e4837255f399af4/Documents/School/Courses/Stat 555/Project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e4837255f399af4/Documents/School/Courses/Stat 555/Project/Stat555Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_F25DC773A252ABDACC104874D15873165ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A573B0-B907-4CAC-B414-DF4CA03A9D04}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="11_F25DC773A252ABDACC104874D15873165ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9DB8C19-D2E7-423E-A533-703A6092D69D}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="6330" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,10 +428,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -721,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -736,10 +732,10 @@
     <col min="8" max="8" width="11.1015625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.3125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.47265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.47265625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.05078125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.9453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.05078125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="73.3125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.68359375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.05078125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.05078125" bestFit="1" customWidth="1"/>

</xml_diff>